<commit_message>
update samples and readme.md
</commit_message>
<xml_diff>
--- a/UnityProject/Assets/Plugins/BakingSheet/Examples/002 - Import From Excel/Excel/Others.xlsx
+++ b/UnityProject/Assets/Plugins/BakingSheet/Examples/002 - Import From Excel/Excel/Others.xlsx
@@ -5,12 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Items" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Monsters" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Dungeons" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Npcs" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -121,6 +123,93 @@
   </si>
   <si>
     <t xml:space="preserve">Dragon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monsters:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monsters:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monsters:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Items:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Items:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DUNGEON001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easy Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DUNGEON002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expert Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DUNGEON003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dragon’s Nest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texts:Greeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texts:Purchasing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texts:Leaving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPC001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fat Baker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morning traveler!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Come again!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPC002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blacksmith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G’day!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good choice.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take care.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPC003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potion Master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What do you want?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take it already.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t come again.</t>
   </si>
 </sst>
 </file>
@@ -132,7 +221,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -167,6 +256,11 @@
       <name val="Helvetica Neue"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Helvetica Neue"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -224,7 +318,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -257,6 +351,14 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -280,11 +382,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.29296875" defaultRowHeight="19.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="19.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.69"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="3" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="3" style="1" width="12.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -523,12 +625,12 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.29296875" defaultRowHeight="19.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="19.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="1" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="1" style="1" width="12.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -655,16 +757,16 @@
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.29296875" defaultRowHeight="19.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="19.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.38"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="8" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="12.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="8" style="1" width="12.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -818,4 +920,214 @@
     <oddFooter>&amp;C&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="24.79"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>